<commit_message>
begin working on new event system
</commit_message>
<xml_diff>
--- a/DocumentationInternal/Lightning2.0RemainingTasks.xlsx
+++ b/DocumentationInternal/Lightning2.0RemainingTasks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FiercePC\Lightning2\DocumentationInternal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8E8E2C-BF55-49E4-AE9E-3B9000F51B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A204C7B-C43D-4FAC-9540-140737FC61AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0BC9E4B3-AF01-4ABE-9665-051385F7AFEC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>January 24, 2023</t>
   </si>
@@ -502,7 +502,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -513,7 +513,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -655,10 +655,16 @@
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="B24" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fontmanager -> static textutils
</commit_message>
<xml_diff>
--- a/DocumentationInternal/Lightning2.0RemainingTasks.xlsx
+++ b/DocumentationInternal/Lightning2.0RemainingTasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FiercePC\Lightning2\DocumentationInternal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A204C7B-C43D-4FAC-9540-140737FC61AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98DAECB2-9F4A-4F05-B267-1F51644254BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0BC9E4B3-AF01-4ABE-9665-051385F7AFEC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>January 24, 2023</t>
   </si>
@@ -510,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9612748B-E59E-4C20-A8D2-F1A4B15171D5}">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="A12" sqref="A12:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -607,7 +607,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -615,17 +615,20 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -633,7 +636,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -641,17 +644,17 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
@@ -659,7 +662,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
@@ -667,27 +670,30 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
fix psrticle effect culling
</commit_message>
<xml_diff>
--- a/DocumentationInternal/Lightning2.0RemainingTasks.xlsx
+++ b/DocumentationInternal/Lightning2.0RemainingTasks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FiercePC\Lightning2\DocumentationInternal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Lightning2\DocumentationInternal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98DAECB2-9F4A-4F05-B267-1F51644254BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7310788-6859-4EB7-A933-ECD19BF249C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0BC9E4B3-AF01-4ABE-9665-051385F7AFEC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0BC9E4B3-AF01-4ABE-9665-051385F7AFEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>January 24, 2023</t>
   </si>
@@ -91,9 +91,6 @@
   </si>
   <si>
     <t>Exhaustive testing of all functionality</t>
-  </si>
-  <si>
-    <t>Better localsettings</t>
   </si>
   <si>
     <t>New API docs</t>
@@ -189,13 +186,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,189 +511,188 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:A14"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="34.28515625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="49.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B4" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B16" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C19" s="6"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix incorrect primitive sizes (off by one) in some circumstances)
</commit_message>
<xml_diff>
--- a/DocumentationInternal/Lightning2.0RemainingTasks.xlsx
+++ b/DocumentationInternal/Lightning2.0RemainingTasks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Lightning2\DocumentationInternal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4FCF365-802F-4DA2-8FEF-45A4D060D1B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3614C52F-7BFA-43EF-AAB9-24C90037C904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0BC9E4B3-AF01-4ABE-9665-051385F7AFEC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0BC9E4B3-AF01-4ABE-9665-051385F7AFEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>January 24, 2023</t>
   </si>
@@ -46,12 +46,6 @@
   </si>
   <si>
     <t>Fix button text positioning</t>
-  </si>
-  <si>
-    <t>Texture Rotation API</t>
-  </si>
-  <si>
-    <t>Multitexture API</t>
   </si>
   <si>
     <t>Fix remaining consistency issues</t>
@@ -505,197 +499,190 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9612748B-E59E-4C20-A8D2-F1A4B15171D5}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="49.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="34.33203125" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="49.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="B19" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="C19" s="6"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="4" t="s">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix off by one error
</commit_message>
<xml_diff>
--- a/DocumentationInternal/Lightning2.0RemainingTasks.xlsx
+++ b/DocumentationInternal/Lightning2.0RemainingTasks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Lightning2\DocumentationInternal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4FCF365-802F-4DA2-8FEF-45A4D060D1B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3614C52F-7BFA-43EF-AAB9-24C90037C904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0BC9E4B3-AF01-4ABE-9665-051385F7AFEC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0BC9E4B3-AF01-4ABE-9665-051385F7AFEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>January 24, 2023</t>
   </si>
@@ -46,12 +46,6 @@
   </si>
   <si>
     <t>Fix button text positioning</t>
-  </si>
-  <si>
-    <t>Texture Rotation API</t>
-  </si>
-  <si>
-    <t>Multitexture API</t>
   </si>
   <si>
     <t>Fix remaining consistency issues</t>
@@ -505,197 +499,190 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9612748B-E59E-4C20-A8D2-F1A4B15171D5}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="49.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="34.33203125" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="49.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="B19" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="C19" s="6"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="4" t="s">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix a bug in basic example
</commit_message>
<xml_diff>
--- a/DocumentationInternal/Lightning2.0RemainingTasks.xlsx
+++ b/DocumentationInternal/Lightning2.0RemainingTasks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Lightning2\DocumentationInternal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Lightning\DocumentationInternal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3614C52F-7BFA-43EF-AAB9-24C90037C904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA6F569-3822-4D37-8FB0-19F76E1533D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0BC9E4B3-AF01-4ABE-9665-051385F7AFEC}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11295" xr2:uid="{0BC9E4B3-AF01-4ABE-9665-051385F7AFEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
-  <si>
-    <t>January 24, 2023</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>Completed</t>
   </si>
@@ -51,15 +48,6 @@
     <t>Fix remaining consistency issues</t>
   </si>
   <si>
-    <t>Bold text</t>
-  </si>
-  <si>
-    <t>Italic text</t>
-  </si>
-  <si>
-    <t>Fix underline / strikethrough text bugs</t>
-  </si>
-  <si>
     <t>Automatically save globalsettings on exit</t>
   </si>
   <si>
@@ -72,9 +60,6 @@
     <t>Renderer-independent blend mode</t>
   </si>
   <si>
-    <t>NativeAOT support</t>
-  </si>
-  <si>
     <t>VS Scene template</t>
   </si>
   <si>
@@ -111,7 +96,7 @@
     <t>Lightning 2.0 Pre-RC Tasks</t>
   </si>
   <si>
-    <t>Partial (DOES NOT WORK YET)</t>
+    <t>Updated March 21, 2023</t>
   </si>
 </sst>
 </file>
@@ -145,7 +130,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -155,12 +140,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -177,14 +156,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9612748B-E59E-4C20-A8D2-F1A4B15171D5}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -514,175 +492,157 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>23</v>
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>23</v>
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>23</v>
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>23</v>
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>23</v>
+        <v>5</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>23</v>
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B11" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>23</v>
+        <v>16</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="6"/>
+      <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>25</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>